<commit_message>
Finish main part of task.
</commit_message>
<xml_diff>
--- a/Contracts Martin Luther/Austria/AGRANA BETEILIGUNGS AG.xlsx
+++ b/Contracts Martin Luther/Austria/AGRANA BETEILIGUNGS AG.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibodia\Desktop\ExcelChecker\Contracts Martin Luther — kopia\Austria\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03DC258-FD17-4BBA-BCCC-BE8421639C66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="20730" windowHeight="6210"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="20730" windowHeight="6210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -51,8 +57,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,8 +126,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -129,14 +135,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -174,9 +183,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,9 +217,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,9 +269,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,16 +462,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +482,7 @@
         <v>0.79600000000000004</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -448,7 +493,7 @@
         <v>2.7400000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -459,7 +504,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -470,18 +515,18 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>368800</v>
+        <v>378800</v>
       </c>
       <c r="C5" s="3">
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -492,7 +537,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -503,7 +548,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -514,7 +559,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -522,10 +567,10 @@
         <v>110800</v>
       </c>
       <c r="C9" s="3">
-        <v>1.8E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -538,7 +583,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.marketscreener.com/SUEDZUCKER-AG-436654/"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.marketscreener.com/SUEDZUCKER-AG-436654/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
@@ -546,24 +591,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>